<commit_message>
update of results and scripts. Anonimyzed fedcore
</commit_message>
<xml_diff>
--- a/results/InceptionNet/AppliancesEnergy/low-rank_quant-dynamic_pruning_quant-qat/0_low-rank_metrics.xlsx
+++ b/results/InceptionNet/AppliancesEnergy/low-rank_quant-dynamic_pruning_quant-qat/0_low-rank_metrics.xlsx
@@ -84,11 +84,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -467,8 +469,8 @@
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="3" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -483,7 +485,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>fedcore</t>
+          <t>approach</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -686,13 +688,13 @@
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="3" t="n"/>
       <c r="E1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="3" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -707,7 +709,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>fedcore</t>
+          <t>approach</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -722,7 +724,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>fedcore</t>
+          <t>approach</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -784,7 +786,6 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">

</xml_diff>